<commit_message>
added case build api spec
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Scenarios1.xlsx
+++ b/src/test/resources/testdata/Scenarios1.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A968A8-B1FB-4737-89EC-CA9330146EF8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65CAE38-140F-4F82-9928-8D254F4E18C5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="355" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2850" yWindow="340" windowWidth="14780" windowHeight="9700" tabRatio="355" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vendors" sheetId="1" r:id="rId1"/>
     <sheet name="CaseBuild" sheetId="2" r:id="rId2"/>
     <sheet name="PartDetails" sheetId="7" r:id="rId3"/>
+    <sheet name="APISpec" sheetId="8" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">Vendors!$A$1:$L$80</definedName>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1483" uniqueCount="203">
   <si>
     <t>TC_ID</t>
   </si>
@@ -316,6 +317,324 @@
   </si>
   <si>
     <t>verifyPartialPurchaseOrderStatus</t>
+  </si>
+  <si>
+    <t>ValidateInvalidVendorCode</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>2020-08-03</t>
+  </si>
+  <si>
+    <t>231231F33</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>2020-08-04</t>
+  </si>
+  <si>
+    <t>231231F34</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>2020-08-05</t>
+  </si>
+  <si>
+    <t>231231F35</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>2020-08-06</t>
+  </si>
+  <si>
+    <t>231231F36</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>2020-08-07</t>
+  </si>
+  <si>
+    <t>231231F37</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>2020-08-08</t>
+  </si>
+  <si>
+    <t>231231F38</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>2020-08-09</t>
+  </si>
+  <si>
+    <t>231231F39</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>2020-08-10</t>
+  </si>
+  <si>
+    <t>231231F40</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>2020-08-11</t>
+  </si>
+  <si>
+    <t>231231F41</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>2020-08-12</t>
+  </si>
+  <si>
+    <t>231231F42</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>2020-08-13</t>
+  </si>
+  <si>
+    <t>231231F43</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>2020-08-14</t>
+  </si>
+  <si>
+    <t>231231F44</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>2020-08-15</t>
+  </si>
+  <si>
+    <t>231231F45</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>2020-08-16</t>
+  </si>
+  <si>
+    <t>231231F46</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>2020-08-17</t>
+  </si>
+  <si>
+    <t>231231F47</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>2020-08-18</t>
+  </si>
+  <si>
+    <t>231231F48</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>2020-08-19</t>
+  </si>
+  <si>
+    <t>231231F49</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>2020-08-20</t>
+  </si>
+  <si>
+    <t>231231F50</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>2020-08-21</t>
+  </si>
+  <si>
+    <t>231231F51</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>2020-08-22</t>
+  </si>
+  <si>
+    <t>231231F52</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>2020-08-23</t>
+  </si>
+  <si>
+    <t>231231F53</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>2020-08-24</t>
+  </si>
+  <si>
+    <t>231231F54</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>2020-08-25</t>
+  </si>
+  <si>
+    <t>231231F55</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>2020-08-26</t>
+  </si>
+  <si>
+    <t>231231F56</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>2020-08-27</t>
+  </si>
+  <si>
+    <t>231231F57</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>2020-08-28</t>
+  </si>
+  <si>
+    <t>231231F58</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>2020-08-29</t>
+  </si>
+  <si>
+    <t>231231F59</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>2020-08-30</t>
+  </si>
+  <si>
+    <t>231231F60</t>
+  </si>
+  <si>
+    <t>ValidateMissingVendorCode</t>
+  </si>
+  <si>
+    <t>ValidateInvalidCaseNumber</t>
+  </si>
+  <si>
+    <t>ValidateInvalidCaseNumberTwice60</t>
+  </si>
+  <si>
+    <t>ValidateMissingCaseNumber</t>
+  </si>
+  <si>
+    <t>ValidateDuplicateCaseNumber</t>
+  </si>
+  <si>
+    <t>ValidateInvalidTransportationCode</t>
+  </si>
+  <si>
+    <t>ValidateRequiredTransportationCode</t>
+  </si>
+  <si>
+    <t>ValidateInvalidDirectShipFlag</t>
+  </si>
+  <si>
+    <t>ValidateMissingDirectShipFlag</t>
+  </si>
+  <si>
+    <t>ValidateDirectShipFlagDealerMissing</t>
+  </si>
+  <si>
+    <t>ValidateInvalidDistFD</t>
+  </si>
+  <si>
+    <t>ValidateMissingDistFD</t>
+  </si>
+  <si>
+    <t>ValidateDealerNumberInvalid</t>
+  </si>
+  <si>
+    <t>ValidateRFIDInvalid</t>
+  </si>
+  <si>
+    <t>ValidateRFIDDuplicate</t>
+  </si>
+  <si>
+    <t>ValidateRFIDTypeInvalid</t>
+  </si>
+  <si>
+    <t>ValidateInvalidPartNumber</t>
+  </si>
+  <si>
+    <t>ValidateMissingPartNumber</t>
+  </si>
+  <si>
+    <t>ValidateDuplicatePartNumber</t>
+  </si>
+  <si>
+    <t>ValidateInvalidPartQuantity</t>
+  </si>
+  <si>
+    <t>ValidateMissingPartQuantity</t>
   </si>
 </sst>
 </file>
@@ -337,12 +656,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -357,9 +682,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -645,7 +972,7 @@
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A10" sqref="A10"/>
-      <selection pane="topRight" activeCell="C5" sqref="C5"/>
+      <selection pane="topRight" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -768,8 +1095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C8715E6-F122-4F08-BC44-70C8316DEBB1}">
   <dimension ref="A1:AC90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2566,9 +2893,89 @@
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A21">
-        <v>10</v>
-      </c>
-      <c r="O21" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
+        <v>95</v>
+      </c>
+      <c r="C21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" t="s">
+        <v>73</v>
+      </c>
+      <c r="H21" t="s">
+        <v>21</v>
+      </c>
+      <c r="I21" t="s">
+        <v>55</v>
+      </c>
+      <c r="J21" t="s">
+        <v>42</v>
+      </c>
+      <c r="K21" t="s">
+        <v>43</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M21" t="s">
+        <v>45</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>76</v>
+      </c>
+      <c r="R21" t="s">
+        <v>74</v>
+      </c>
+      <c r="S21" t="s">
+        <v>49</v>
+      </c>
+      <c r="T21" t="s">
+        <v>77</v>
+      </c>
+      <c r="U21" t="s">
+        <v>50</v>
+      </c>
+      <c r="V21" t="s">
+        <v>51</v>
+      </c>
+      <c r="W21" t="s">
+        <v>52</v>
+      </c>
+      <c r="X21" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A22">
@@ -2668,4 +3075,2811 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59B65348-517C-47CA-8285-606378C5A9F1}">
+  <dimension ref="A1:AC33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:XFD23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="5.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="29.36328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="28.36328125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="30.81640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="28.1796875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="30.1796875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.54296875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>34</v>
+      </c>
+      <c r="R1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S1" t="s">
+        <v>36</v>
+      </c>
+      <c r="T1" t="s">
+        <v>63</v>
+      </c>
+      <c r="U1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V1" t="s">
+        <v>38</v>
+      </c>
+      <c r="W1" t="s">
+        <v>39</v>
+      </c>
+      <c r="X1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>76</v>
+      </c>
+      <c r="R2" t="s">
+        <v>74</v>
+      </c>
+      <c r="S2" t="s">
+        <v>49</v>
+      </c>
+      <c r="T2" t="s">
+        <v>77</v>
+      </c>
+      <c r="U2" t="s">
+        <v>50</v>
+      </c>
+      <c r="V2" t="s">
+        <v>51</v>
+      </c>
+      <c r="W2" t="s">
+        <v>52</v>
+      </c>
+      <c r="X2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" t="s">
+        <v>43</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M3" t="s">
+        <v>45</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>76</v>
+      </c>
+      <c r="R3" t="s">
+        <v>74</v>
+      </c>
+      <c r="S3" t="s">
+        <v>49</v>
+      </c>
+      <c r="T3" t="s">
+        <v>77</v>
+      </c>
+      <c r="U3" t="s">
+        <v>50</v>
+      </c>
+      <c r="V3" t="s">
+        <v>51</v>
+      </c>
+      <c r="W3" t="s">
+        <v>52</v>
+      </c>
+      <c r="X3" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M4" t="s">
+        <v>45</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>76</v>
+      </c>
+      <c r="R4" t="s">
+        <v>74</v>
+      </c>
+      <c r="S4" t="s">
+        <v>49</v>
+      </c>
+      <c r="T4" t="s">
+        <v>77</v>
+      </c>
+      <c r="U4" t="s">
+        <v>50</v>
+      </c>
+      <c r="V4" t="s">
+        <v>51</v>
+      </c>
+      <c r="W4" t="s">
+        <v>52</v>
+      </c>
+      <c r="X4" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" s="2" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="X5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y5" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC5" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" s="2" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="U6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="V6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y6" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z6" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB6" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC6" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J7" t="s">
+        <v>42</v>
+      </c>
+      <c r="K7" t="s">
+        <v>43</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="M7" t="s">
+        <v>45</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>76</v>
+      </c>
+      <c r="R7" t="s">
+        <v>74</v>
+      </c>
+      <c r="S7" t="s">
+        <v>49</v>
+      </c>
+      <c r="T7" t="s">
+        <v>77</v>
+      </c>
+      <c r="U7" t="s">
+        <v>50</v>
+      </c>
+      <c r="V7" t="s">
+        <v>51</v>
+      </c>
+      <c r="W7" t="s">
+        <v>52</v>
+      </c>
+      <c r="X7" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" s="2" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="U8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="V8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="W8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="X8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA8" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC8" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>187</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" t="s">
+        <v>73</v>
+      </c>
+      <c r="H9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" t="s">
+        <v>55</v>
+      </c>
+      <c r="J9" t="s">
+        <v>42</v>
+      </c>
+      <c r="K9" t="s">
+        <v>43</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="M9" t="s">
+        <v>45</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>76</v>
+      </c>
+      <c r="R9" t="s">
+        <v>74</v>
+      </c>
+      <c r="S9" t="s">
+        <v>49</v>
+      </c>
+      <c r="T9" t="s">
+        <v>77</v>
+      </c>
+      <c r="U9" t="s">
+        <v>50</v>
+      </c>
+      <c r="V9" t="s">
+        <v>51</v>
+      </c>
+      <c r="W9" t="s">
+        <v>52</v>
+      </c>
+      <c r="X9" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" s="2" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="V10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="W10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="X10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA10" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC10" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>189</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11" t="s">
+        <v>73</v>
+      </c>
+      <c r="H11" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" t="s">
+        <v>55</v>
+      </c>
+      <c r="J11" t="s">
+        <v>42</v>
+      </c>
+      <c r="K11" t="s">
+        <v>43</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="M11" t="s">
+        <v>45</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>76</v>
+      </c>
+      <c r="R11" t="s">
+        <v>74</v>
+      </c>
+      <c r="S11" t="s">
+        <v>49</v>
+      </c>
+      <c r="T11" t="s">
+        <v>77</v>
+      </c>
+      <c r="U11" t="s">
+        <v>50</v>
+      </c>
+      <c r="V11" t="s">
+        <v>51</v>
+      </c>
+      <c r="W11" t="s">
+        <v>52</v>
+      </c>
+      <c r="X11" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>190</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" t="s">
+        <v>72</v>
+      </c>
+      <c r="F12" t="s">
+        <v>73</v>
+      </c>
+      <c r="H12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" t="s">
+        <v>55</v>
+      </c>
+      <c r="J12" t="s">
+        <v>42</v>
+      </c>
+      <c r="K12" t="s">
+        <v>43</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="M12" t="s">
+        <v>45</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>76</v>
+      </c>
+      <c r="R12" t="s">
+        <v>74</v>
+      </c>
+      <c r="S12" t="s">
+        <v>49</v>
+      </c>
+      <c r="T12" t="s">
+        <v>77</v>
+      </c>
+      <c r="U12" t="s">
+        <v>50</v>
+      </c>
+      <c r="V12" t="s">
+        <v>51</v>
+      </c>
+      <c r="W12" t="s">
+        <v>52</v>
+      </c>
+      <c r="X12" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>191</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" t="s">
+        <v>73</v>
+      </c>
+      <c r="H13" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" t="s">
+        <v>55</v>
+      </c>
+      <c r="J13" t="s">
+        <v>42</v>
+      </c>
+      <c r="K13" t="s">
+        <v>43</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M13" t="s">
+        <v>45</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>76</v>
+      </c>
+      <c r="R13" t="s">
+        <v>74</v>
+      </c>
+      <c r="S13" t="s">
+        <v>49</v>
+      </c>
+      <c r="T13" t="s">
+        <v>77</v>
+      </c>
+      <c r="U13" t="s">
+        <v>50</v>
+      </c>
+      <c r="V13" t="s">
+        <v>51</v>
+      </c>
+      <c r="W13" t="s">
+        <v>52</v>
+      </c>
+      <c r="X13" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+    </row>
+    <row r="15" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>192</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" t="s">
+        <v>73</v>
+      </c>
+      <c r="H15" t="s">
+        <v>21</v>
+      </c>
+      <c r="I15" t="s">
+        <v>55</v>
+      </c>
+      <c r="J15" t="s">
+        <v>42</v>
+      </c>
+      <c r="K15" t="s">
+        <v>43</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="M15" t="s">
+        <v>45</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>76</v>
+      </c>
+      <c r="R15" t="s">
+        <v>74</v>
+      </c>
+      <c r="S15" t="s">
+        <v>49</v>
+      </c>
+      <c r="T15" t="s">
+        <v>77</v>
+      </c>
+      <c r="U15" t="s">
+        <v>50</v>
+      </c>
+      <c r="V15" t="s">
+        <v>51</v>
+      </c>
+      <c r="W15" t="s">
+        <v>52</v>
+      </c>
+      <c r="X15" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>193</v>
+      </c>
+      <c r="C16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" t="s">
+        <v>73</v>
+      </c>
+      <c r="H16" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16" t="s">
+        <v>55</v>
+      </c>
+      <c r="J16" t="s">
+        <v>42</v>
+      </c>
+      <c r="K16" t="s">
+        <v>43</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="M16" t="s">
+        <v>45</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>76</v>
+      </c>
+      <c r="R16" t="s">
+        <v>74</v>
+      </c>
+      <c r="S16" t="s">
+        <v>49</v>
+      </c>
+      <c r="T16" t="s">
+        <v>77</v>
+      </c>
+      <c r="U16" t="s">
+        <v>50</v>
+      </c>
+      <c r="V16" t="s">
+        <v>51</v>
+      </c>
+      <c r="W16" t="s">
+        <v>52</v>
+      </c>
+      <c r="X16" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>194</v>
+      </c>
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" t="s">
+        <v>73</v>
+      </c>
+      <c r="H17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17" t="s">
+        <v>55</v>
+      </c>
+      <c r="J17" t="s">
+        <v>42</v>
+      </c>
+      <c r="K17" t="s">
+        <v>43</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="M17" t="s">
+        <v>45</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>76</v>
+      </c>
+      <c r="R17" t="s">
+        <v>74</v>
+      </c>
+      <c r="S17" t="s">
+        <v>49</v>
+      </c>
+      <c r="T17" t="s">
+        <v>77</v>
+      </c>
+      <c r="U17" t="s">
+        <v>50</v>
+      </c>
+      <c r="V17" t="s">
+        <v>51</v>
+      </c>
+      <c r="W17" t="s">
+        <v>52</v>
+      </c>
+      <c r="X17" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" s="2" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="2">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N18" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="O18" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="P18" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q18" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="R18" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="S18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="T18" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="U18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="V18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="W18" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="X18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y18" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z18" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA18" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB18" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC18" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" s="2" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="2">
+        <v>17</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N19" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="O19" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="P19" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q19" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="R19" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="S19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="T19" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="U19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="V19" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="W19" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="X19" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y19" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z19" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA19" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB19" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC19" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" s="2" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="2">
+        <v>18</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N20" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="O20" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="P20" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q20" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="R20" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="S20" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="T20" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="U20" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="V20" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="W20" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="X20" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y20" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z20" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA20" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB20" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC20" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>198</v>
+      </c>
+      <c r="C21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" t="s">
+        <v>73</v>
+      </c>
+      <c r="H21" t="s">
+        <v>21</v>
+      </c>
+      <c r="I21" t="s">
+        <v>55</v>
+      </c>
+      <c r="J21" t="s">
+        <v>42</v>
+      </c>
+      <c r="K21" t="s">
+        <v>43</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="M21" t="s">
+        <v>45</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>76</v>
+      </c>
+      <c r="R21" t="s">
+        <v>74</v>
+      </c>
+      <c r="S21" t="s">
+        <v>49</v>
+      </c>
+      <c r="T21" t="s">
+        <v>77</v>
+      </c>
+      <c r="U21" t="s">
+        <v>50</v>
+      </c>
+      <c r="V21" t="s">
+        <v>51</v>
+      </c>
+      <c r="W21" t="s">
+        <v>52</v>
+      </c>
+      <c r="X21" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>199</v>
+      </c>
+      <c r="C22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" t="s">
+        <v>72</v>
+      </c>
+      <c r="F22" t="s">
+        <v>73</v>
+      </c>
+      <c r="H22" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22" t="s">
+        <v>55</v>
+      </c>
+      <c r="J22" t="s">
+        <v>42</v>
+      </c>
+      <c r="K22" t="s">
+        <v>43</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="M22" t="s">
+        <v>45</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>76</v>
+      </c>
+      <c r="R22" t="s">
+        <v>74</v>
+      </c>
+      <c r="S22" t="s">
+        <v>49</v>
+      </c>
+      <c r="T22" t="s">
+        <v>77</v>
+      </c>
+      <c r="U22" t="s">
+        <v>50</v>
+      </c>
+      <c r="V22" t="s">
+        <v>51</v>
+      </c>
+      <c r="W22" t="s">
+        <v>52</v>
+      </c>
+      <c r="X22" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" s="2" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="2">
+        <v>21</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N23" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="O23" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="P23" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q23" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="R23" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="S23" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="T23" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="U23" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="V23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="W23" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="X23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y23" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z23" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA23" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB23" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC23" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>201</v>
+      </c>
+      <c r="C24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" t="s">
+        <v>20</v>
+      </c>
+      <c r="E24" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24" t="s">
+        <v>73</v>
+      </c>
+      <c r="H24" t="s">
+        <v>21</v>
+      </c>
+      <c r="I24" t="s">
+        <v>55</v>
+      </c>
+      <c r="J24" t="s">
+        <v>42</v>
+      </c>
+      <c r="K24" t="s">
+        <v>43</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="M24" t="s">
+        <v>45</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>76</v>
+      </c>
+      <c r="R24" t="s">
+        <v>74</v>
+      </c>
+      <c r="S24" t="s">
+        <v>49</v>
+      </c>
+      <c r="T24" t="s">
+        <v>77</v>
+      </c>
+      <c r="U24" t="s">
+        <v>50</v>
+      </c>
+      <c r="V24" t="s">
+        <v>51</v>
+      </c>
+      <c r="W24" t="s">
+        <v>52</v>
+      </c>
+      <c r="X24" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>202</v>
+      </c>
+      <c r="C25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" t="s">
+        <v>72</v>
+      </c>
+      <c r="F25" t="s">
+        <v>73</v>
+      </c>
+      <c r="H25" t="s">
+        <v>21</v>
+      </c>
+      <c r="I25" t="s">
+        <v>55</v>
+      </c>
+      <c r="J25" t="s">
+        <v>42</v>
+      </c>
+      <c r="K25" t="s">
+        <v>43</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="M25" t="s">
+        <v>45</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>76</v>
+      </c>
+      <c r="R25" t="s">
+        <v>74</v>
+      </c>
+      <c r="S25" t="s">
+        <v>49</v>
+      </c>
+      <c r="T25" t="s">
+        <v>77</v>
+      </c>
+      <c r="U25" t="s">
+        <v>50</v>
+      </c>
+      <c r="V25" t="s">
+        <v>51</v>
+      </c>
+      <c r="W25" t="s">
+        <v>52</v>
+      </c>
+      <c r="X25" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>97</v>
+      </c>
+      <c r="C26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" t="s">
+        <v>20</v>
+      </c>
+      <c r="E26" t="s">
+        <v>72</v>
+      </c>
+      <c r="F26" t="s">
+        <v>73</v>
+      </c>
+      <c r="H26" t="s">
+        <v>21</v>
+      </c>
+      <c r="I26" t="s">
+        <v>55</v>
+      </c>
+      <c r="J26" t="s">
+        <v>42</v>
+      </c>
+      <c r="K26" t="s">
+        <v>43</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="M26" t="s">
+        <v>45</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>76</v>
+      </c>
+      <c r="R26" t="s">
+        <v>74</v>
+      </c>
+      <c r="S26" t="s">
+        <v>49</v>
+      </c>
+      <c r="T26" t="s">
+        <v>77</v>
+      </c>
+      <c r="U26" t="s">
+        <v>50</v>
+      </c>
+      <c r="V26" t="s">
+        <v>51</v>
+      </c>
+      <c r="W26" t="s">
+        <v>52</v>
+      </c>
+      <c r="X26" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC26" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>97</v>
+      </c>
+      <c r="C27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" t="s">
+        <v>72</v>
+      </c>
+      <c r="F27" t="s">
+        <v>73</v>
+      </c>
+      <c r="H27" t="s">
+        <v>21</v>
+      </c>
+      <c r="I27" t="s">
+        <v>55</v>
+      </c>
+      <c r="J27" t="s">
+        <v>42</v>
+      </c>
+      <c r="K27" t="s">
+        <v>43</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="M27" t="s">
+        <v>45</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>76</v>
+      </c>
+      <c r="R27" t="s">
+        <v>74</v>
+      </c>
+      <c r="S27" t="s">
+        <v>49</v>
+      </c>
+      <c r="T27" t="s">
+        <v>77</v>
+      </c>
+      <c r="U27" t="s">
+        <v>50</v>
+      </c>
+      <c r="V27" t="s">
+        <v>51</v>
+      </c>
+      <c r="W27" t="s">
+        <v>52</v>
+      </c>
+      <c r="X27" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC27" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>97</v>
+      </c>
+      <c r="C28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" t="s">
+        <v>20</v>
+      </c>
+      <c r="E28" t="s">
+        <v>72</v>
+      </c>
+      <c r="F28" t="s">
+        <v>73</v>
+      </c>
+      <c r="H28" t="s">
+        <v>21</v>
+      </c>
+      <c r="I28" t="s">
+        <v>55</v>
+      </c>
+      <c r="J28" t="s">
+        <v>42</v>
+      </c>
+      <c r="K28" t="s">
+        <v>43</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="M28" t="s">
+        <v>45</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>76</v>
+      </c>
+      <c r="R28" t="s">
+        <v>74</v>
+      </c>
+      <c r="S28" t="s">
+        <v>49</v>
+      </c>
+      <c r="T28" t="s">
+        <v>77</v>
+      </c>
+      <c r="U28" t="s">
+        <v>50</v>
+      </c>
+      <c r="V28" t="s">
+        <v>51</v>
+      </c>
+      <c r="W28" t="s">
+        <v>52</v>
+      </c>
+      <c r="X28" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC28" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>97</v>
+      </c>
+      <c r="C29" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" t="s">
+        <v>20</v>
+      </c>
+      <c r="E29" t="s">
+        <v>72</v>
+      </c>
+      <c r="F29" t="s">
+        <v>73</v>
+      </c>
+      <c r="H29" t="s">
+        <v>21</v>
+      </c>
+      <c r="I29" t="s">
+        <v>55</v>
+      </c>
+      <c r="J29" t="s">
+        <v>42</v>
+      </c>
+      <c r="K29" t="s">
+        <v>43</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="M29" t="s">
+        <v>45</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>76</v>
+      </c>
+      <c r="R29" t="s">
+        <v>74</v>
+      </c>
+      <c r="S29" t="s">
+        <v>49</v>
+      </c>
+      <c r="T29" t="s">
+        <v>77</v>
+      </c>
+      <c r="U29" t="s">
+        <v>50</v>
+      </c>
+      <c r="V29" t="s">
+        <v>51</v>
+      </c>
+      <c r="W29" t="s">
+        <v>52</v>
+      </c>
+      <c r="X29" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC29" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>97</v>
+      </c>
+      <c r="C30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" t="s">
+        <v>20</v>
+      </c>
+      <c r="E30" t="s">
+        <v>72</v>
+      </c>
+      <c r="F30" t="s">
+        <v>73</v>
+      </c>
+      <c r="H30" t="s">
+        <v>21</v>
+      </c>
+      <c r="I30" t="s">
+        <v>55</v>
+      </c>
+      <c r="J30" t="s">
+        <v>42</v>
+      </c>
+      <c r="K30" t="s">
+        <v>43</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="M30" t="s">
+        <v>45</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>76</v>
+      </c>
+      <c r="R30" t="s">
+        <v>74</v>
+      </c>
+      <c r="S30" t="s">
+        <v>49</v>
+      </c>
+      <c r="T30" t="s">
+        <v>77</v>
+      </c>
+      <c r="U30" t="s">
+        <v>50</v>
+      </c>
+      <c r="V30" t="s">
+        <v>51</v>
+      </c>
+      <c r="W30" t="s">
+        <v>52</v>
+      </c>
+      <c r="X30" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC30" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>97</v>
+      </c>
+      <c r="C31" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" t="s">
+        <v>20</v>
+      </c>
+      <c r="E31" t="s">
+        <v>72</v>
+      </c>
+      <c r="F31" t="s">
+        <v>73</v>
+      </c>
+      <c r="H31" t="s">
+        <v>21</v>
+      </c>
+      <c r="I31" t="s">
+        <v>55</v>
+      </c>
+      <c r="J31" t="s">
+        <v>42</v>
+      </c>
+      <c r="K31" t="s">
+        <v>43</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="M31" t="s">
+        <v>45</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="P31" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>76</v>
+      </c>
+      <c r="R31" t="s">
+        <v>74</v>
+      </c>
+      <c r="S31" t="s">
+        <v>49</v>
+      </c>
+      <c r="T31" t="s">
+        <v>77</v>
+      </c>
+      <c r="U31" t="s">
+        <v>50</v>
+      </c>
+      <c r="V31" t="s">
+        <v>51</v>
+      </c>
+      <c r="W31" t="s">
+        <v>52</v>
+      </c>
+      <c r="X31" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z31" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA31" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB31" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC31" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>97</v>
+      </c>
+      <c r="C32" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" t="s">
+        <v>20</v>
+      </c>
+      <c r="E32" t="s">
+        <v>72</v>
+      </c>
+      <c r="F32" t="s">
+        <v>73</v>
+      </c>
+      <c r="H32" t="s">
+        <v>21</v>
+      </c>
+      <c r="I32" t="s">
+        <v>55</v>
+      </c>
+      <c r="J32" t="s">
+        <v>42</v>
+      </c>
+      <c r="K32" t="s">
+        <v>43</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="M32" t="s">
+        <v>45</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="P32" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>76</v>
+      </c>
+      <c r="R32" t="s">
+        <v>74</v>
+      </c>
+      <c r="S32" t="s">
+        <v>49</v>
+      </c>
+      <c r="T32" t="s">
+        <v>77</v>
+      </c>
+      <c r="U32" t="s">
+        <v>50</v>
+      </c>
+      <c r="V32" t="s">
+        <v>51</v>
+      </c>
+      <c r="W32" t="s">
+        <v>52</v>
+      </c>
+      <c r="X32" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB32" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" t="s">
+        <v>20</v>
+      </c>
+      <c r="E33" t="s">
+        <v>72</v>
+      </c>
+      <c r="F33" t="s">
+        <v>73</v>
+      </c>
+      <c r="H33" t="s">
+        <v>21</v>
+      </c>
+      <c r="I33" t="s">
+        <v>55</v>
+      </c>
+      <c r="J33" t="s">
+        <v>42</v>
+      </c>
+      <c r="K33" t="s">
+        <v>43</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="M33" t="s">
+        <v>45</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="O33" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="P33" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>76</v>
+      </c>
+      <c r="R33" t="s">
+        <v>74</v>
+      </c>
+      <c r="S33" t="s">
+        <v>49</v>
+      </c>
+      <c r="T33" t="s">
+        <v>77</v>
+      </c>
+      <c r="U33" t="s">
+        <v>50</v>
+      </c>
+      <c r="V33" t="s">
+        <v>51</v>
+      </c>
+      <c r="W33" t="s">
+        <v>52</v>
+      </c>
+      <c r="X33" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC33" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>